<commit_message>
how tf is adx test passing and tr update alone failing HUH?
</commit_message>
<xml_diff>
--- a/resources/btc-adx.xlsx
+++ b/resources/btc-adx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944BE0FA-FBEF-4545-94B9-DDAF08CC98FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF7110F-9ADE-4449-8412-5BCA701DB450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-8955" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,13 +369,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29:P200"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1515669120</v>
       </c>
@@ -396,8 +392,41 @@
         <f>B1-C1</f>
         <v>56.799999999999272</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1515669180</v>
       </c>
@@ -412,6 +441,9 @@
       </c>
       <c r="E2">
         <f>MAX(B2-C2,ABS(B2-D1),ABS(D1-C2))</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
@@ -430,8 +462,26 @@
         <f>IF(AND(H2&gt;G2,H2&gt;0),H2,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1515669240</v>
       </c>
@@ -448,6 +498,9 @@
         <f t="shared" ref="E3:E66" si="0">MAX(B3-C3,ABS(B3-D2),ABS(D2-C3))</f>
         <v>50.299999999999272</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" si="1">B3-B2</f>
         <v>50.299999999999272</v>
@@ -464,8 +517,26 @@
         <f t="shared" ref="J3:J66" si="4">IF(AND(H3&gt;G3,H3&gt;0),H3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1515669300</v>
       </c>
@@ -482,6 +553,9 @@
         <f t="shared" si="0"/>
         <v>9.9999999998544808E-2</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="G4">
         <f t="shared" si="1"/>
         <v>-23</v>
@@ -498,8 +572,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1515669360</v>
       </c>
@@ -516,6 +608,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -532,8 +627,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1515669420</v>
       </c>
@@ -550,6 +663,9 @@
         <f t="shared" si="0"/>
         <v>73.299999999999272</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="G6">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -566,8 +682,26 @@
         <f t="shared" si="4"/>
         <v>73.299999999999272</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1515669480</v>
       </c>
@@ -584,6 +718,9 @@
         <f t="shared" si="0"/>
         <v>22.099999999998545</v>
       </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
       <c r="G7">
         <f t="shared" si="1"/>
         <v>-66</v>
@@ -600,8 +737,26 @@
         <f t="shared" si="4"/>
         <v>14.799999999999272</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1515669540</v>
       </c>
@@ -618,6 +773,9 @@
         <f t="shared" si="0"/>
         <v>44.799999999999272</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="G8">
         <f t="shared" si="1"/>
         <v>-5.5</v>
@@ -634,8 +792,26 @@
         <f t="shared" si="4"/>
         <v>28.200000000000728</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1515669600</v>
       </c>
@@ -652,6 +828,9 @@
         <f t="shared" si="0"/>
         <v>81.899999999999636</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="G9">
         <f t="shared" si="1"/>
         <v>37.100000000000364</v>
@@ -668,8 +847,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1515669660</v>
       </c>
@@ -686,6 +883,9 @@
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="G10">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -702,8 +902,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1515669720</v>
       </c>
@@ -720,6 +938,9 @@
         <f t="shared" si="0"/>
         <v>33.799999999999272</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>-17.5</v>
@@ -736,8 +957,26 @@
         <f t="shared" si="4"/>
         <v>13.799999999999272</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1515669780</v>
       </c>
@@ -754,6 +993,9 @@
         <f t="shared" si="0"/>
         <v>53.800000000001091</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="G12">
         <f t="shared" si="1"/>
         <v>53.800000000001091</v>
@@ -770,8 +1012,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1515669840</v>
       </c>
@@ -788,6 +1048,9 @@
         <f t="shared" si="0"/>
         <v>17.899999999999636</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
       <c r="G13">
         <f t="shared" si="1"/>
         <v>17.699999999998909</v>
@@ -804,8 +1067,26 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1515669900</v>
       </c>
@@ -822,6 +1103,9 @@
         <f t="shared" si="0"/>
         <v>29.200000000000728</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="G14">
         <f t="shared" si="1"/>
         <v>-17.899999999999636</v>
@@ -838,8 +1122,26 @@
         <f t="shared" si="4"/>
         <v>29.200000000000728</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1515669960</v>
       </c>
@@ -896,8 +1198,11 @@
         <f>(ABS(M15-N15)/SUM(M15,N15))*100</f>
         <v>2.7837259100638145</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1515670020</v>
       </c>
@@ -954,6 +1259,9 @@
         <f t="shared" ref="O16:O79" si="7">(ABS(M16-N16)/SUM(M16,N16))*100</f>
         <v>2.2783150303224717</v>
       </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1012,6 +1320,9 @@
         <f t="shared" si="7"/>
         <v>2.2783150303224713</v>
       </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1070,6 +1381,9 @@
         <f t="shared" si="7"/>
         <v>6.954501619491281</v>
       </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1128,6 +1442,9 @@
         <f t="shared" si="7"/>
         <v>3.8921639486492006</v>
       </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1186,6 +1503,9 @@
         <f t="shared" si="7"/>
         <v>3.8921639486491917</v>
       </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1244,6 +1564,9 @@
         <f t="shared" si="7"/>
         <v>3.8921639486491806</v>
       </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1302,6 +1625,9 @@
         <f t="shared" si="7"/>
         <v>21.618515324338023</v>
       </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1360,6 +1686,9 @@
         <f t="shared" si="7"/>
         <v>43.352704535782728</v>
       </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1418,6 +1747,9 @@
         <f t="shared" si="7"/>
         <v>43.352704535782721</v>
       </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1476,6 +1808,9 @@
         <f t="shared" si="7"/>
         <v>47.474561364896644</v>
       </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1534,6 +1869,9 @@
         <f t="shared" si="7"/>
         <v>51.138238322752848</v>
       </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1591,6 +1929,9 @@
       <c r="O27">
         <f t="shared" si="7"/>
         <v>52.341328353454884</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>